<commit_message>
add write_excel and youhua
</commit_message>
<xml_diff>
--- a/Meizhu/meizhu_testcase.xlsx
+++ b/Meizhu/meizhu_testcase.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" windowHeight="7950" windowWidth="14805" xWindow="240" yWindow="165"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="美住登录" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="间夜房-提交订单" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="美住登录" sheetId="1" r:id="rId1"/>
+    <sheet name="间夜房-提交订单" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" concurrentCalc="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>用户名</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>密码不正确</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>18802094000</t>
@@ -87,61 +84,60 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <family val="3"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <family val="3"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <family val="3"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <family val="3"/>
-      <color rgb="FF222222"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <family val="2"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <family val="3"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -163,24 +159,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -470,23 +472,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="18.125"/>
-    <col customWidth="1" max="2" min="2" width="22.75"/>
-    <col customWidth="1" max="3" min="3" width="35.875"/>
-    <col customWidth="1" max="4" min="4" width="19.875"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="22.75" customWidth="1"/>
+    <col min="3" max="3" width="35.875" customWidth="1"/>
+    <col min="4" max="4" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -513,22 +511,16 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -536,61 +528,46 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="n"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1" t="n"/>
+      <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -598,58 +575,52 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="n"/>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1" t="n"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="17.125"/>
-    <col customWidth="1" max="2" min="2" width="20.875"/>
-    <col customWidth="1" max="3" min="3" width="28.625"/>
-    <col customWidth="1" max="4" min="4" width="13.125"/>
-    <col customWidth="1" max="5" min="5" width="12.625"/>
-    <col customWidth="1" max="6" min="6" width="35.25"/>
-    <col customWidth="1" max="7" min="7" width="25.75"/>
+    <col min="1" max="1" width="17.125" customWidth="1"/>
+    <col min="2" max="2" width="20.875" customWidth="1"/>
+    <col min="3" max="3" width="28.625" customWidth="1"/>
+    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="5" max="5" width="12.625" customWidth="1"/>
+    <col min="6" max="6" width="35.25" customWidth="1"/>
+    <col min="7" max="7" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>2</v>
@@ -659,24 +630,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>